<commit_message>
Actualizar plantilla en atención del INC 2024-001674
</commit_message>
<xml_diff>
--- a/SIGOFCv3/Archivos/Plantilla/CapacitacionParticipantes_v3.xlsx
+++ b/SIGOFCv3/Archivos/Plantilla/CapacitacionParticipantes_v3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20405"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64406F25-26B5-4C9B-B28A-5E4B06DA583F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC62A2F8-3028-412D-A566-1CEB651497CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="1944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2020" uniqueCount="1945">
   <si>
     <t>OBSERVACION</t>
   </si>
@@ -5587,9 +5587,6 @@
     <t>San Jose de Sarapanga (LORETO-MAYNAS-NAUTA)</t>
   </si>
   <si>
-    <t>Murui-Muinani (LORETO-PUTUMAYO-BELETENIENTE MANUEL CLAVERON)</t>
-  </si>
-  <si>
     <t>8 de diciembre (LORETO-PUTUMAYO-PUTUMAYO)</t>
   </si>
   <si>
@@ -5861,6 +5858,12 @@
   </si>
   <si>
     <t>Nueva Unión (UCAYALI-CORONEL PORTILLO-IPARÍA)</t>
+  </si>
+  <si>
+    <t>Murui-Muinani (LORETO-PUTUMAYO-TENIENTE MANUEL CLAVERO)</t>
+  </si>
+  <si>
+    <t>San Martin de Porres (LORETO-PUTUMAYO-TENIENTE MANUEL CLAVERO)</t>
   </si>
 </sst>
 </file>
@@ -6390,7 +6393,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Dato inválido" error="Seleccione del listado" xr:uid="{ECCC55BC-FDD7-4FAC-94A4-9DBC5452FD9D}">
           <x14:formula1>
-            <xm:f>Hoja3!$C$1:$C$1760</xm:f>
+            <xm:f>Hoja3!$C$1:$C$1762</xm:f>
           </x14:formula1>
           <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
@@ -6402,9 +6405,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E1760"/>
+  <dimension ref="A1:E1761"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A1722" workbookViewId="0">
+      <selection activeCell="C1117" sqref="C1117"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12371,432 +12376,432 @@
     </row>
     <row r="1115" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1115" t="s">
-        <v>1873</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="1116" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1116" t="s">
-        <v>1874</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="1117" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1117" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="1118" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1118" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="1119" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1119" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="1120" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1120" t="s">
-        <v>1133</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="1121" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1121" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="1122" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1122" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="1123" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1123" t="s">
-        <v>1878</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="1124" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1124" t="s">
-        <v>1879</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="1125" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1125" t="s">
-        <v>1135</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="1126" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1126" t="s">
-        <v>1880</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="1127" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1127" t="s">
-        <v>1881</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="1128" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1128" t="s">
-        <v>1136</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="1129" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1129" t="s">
-        <v>1882</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="1130" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1130" t="s">
-        <v>1883</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="1131" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1131" t="s">
-        <v>1137</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="1132" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1132" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="1133" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1133" t="s">
-        <v>1884</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="1134" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1134" t="s">
-        <v>1139</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="1135" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1135" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="1136" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1136" t="s">
-        <v>1885</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="1137" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1137" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="1138" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1138" t="s">
-        <v>1887</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="1139" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1139" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="1140" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1140" t="s">
-        <v>1889</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1141" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1141" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="1142" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1142" t="s">
-        <v>1891</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="1143" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1143" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="1144" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1144" t="s">
-        <v>1893</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="1145" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1145" t="s">
-        <v>1894</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="1146" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1146" t="s">
-        <v>1895</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="1147" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1147" t="s">
-        <v>1896</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="1148" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1148" t="s">
-        <v>1897</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="1149" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1149" t="s">
-        <v>1898</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="1150" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1150" t="s">
-        <v>1899</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="1151" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1151" t="s">
-        <v>1141</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="1152" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1152" t="s">
-        <v>1900</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="1153" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1153" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="1154" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1154" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="1155" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1155" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="1156" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1156" t="s">
-        <v>1904</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="1157" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1157" t="s">
-        <v>1905</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="1158" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1158" t="s">
-        <v>1906</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="1159" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1159" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="1160" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1160" t="s">
-        <v>1908</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="1161" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1161" t="s">
-        <v>1909</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="1162" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1162" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="1163" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1163" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="1164" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1164" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="1165" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1165" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="1166" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1166" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="1167" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1167" t="s">
-        <v>1912</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="1168" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1168" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="1169" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1169" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="1170" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1170" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="1171" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1171" t="s">
-        <v>1142</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="1172" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1172" t="s">
-        <v>1916</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="1173" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1173" t="s">
-        <v>1143</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="1174" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1174" t="s">
-        <v>1917</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="1175" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1175" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="1176" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1176" t="s">
-        <v>1144</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="1177" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1177" t="s">
-        <v>1919</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="1178" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1178" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="1179" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1179" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="1180" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1180" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="1181" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1181" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="1182" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1182" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="1183" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1183" t="s">
-        <v>1146</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="1184" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1184" t="s">
-        <v>1924</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="1185" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1185" t="s">
-        <v>1145</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="1186" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1186" t="s">
-        <v>1925</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="1187" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1187" t="s">
-        <v>1147</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="1188" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1188" t="s">
-        <v>1926</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="1189" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1189" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="1190" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1190" t="s">
-        <v>1148</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="1191" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1191" t="s">
-        <v>1928</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1192" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1192" t="s">
-        <v>1149</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="1193" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1193" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="1194" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1194" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1195" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1195" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1196" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1196" t="s">
-        <v>1929</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="1197" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1197" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="1198" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1198" t="s">
-        <v>1153</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="1199" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1199" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="1200" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1200" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="1201" spans="3:3" x14ac:dyDescent="0.3">
@@ -12806,2796 +12811,2801 @@
     </row>
     <row r="1202" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1202" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="1203" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1203" t="s">
-        <v>1155</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="1204" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1204" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="1205" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1205" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="1206" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1206" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="1207" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1207" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="1208" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1208" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="1209" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1209" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="1210" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1210" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="1211" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1211" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="1212" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1212" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="1213" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1213" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="1214" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1214" t="s">
-        <v>1166</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="1215" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1215" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="1216" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1216" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="1217" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1217" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="1218" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1218" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="1219" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1219" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="1220" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1220" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="1221" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1221" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="1222" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1222" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="1223" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1223" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="1224" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1224" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="1225" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1225" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="1226" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1226" t="s">
-        <v>1177</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1227" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1227" t="s">
-        <v>1180</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="1228" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1228" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1229" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1229" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="1230" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1230" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="1231" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1231" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="1232" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1232" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="1233" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1233" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="1234" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1234" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="1235" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1235" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="1236" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1236" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="1237" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1237" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="1238" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1238" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="1239" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1239" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="1240" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1240" t="s">
-        <v>1931</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="1241" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1241" t="s">
-        <v>1194</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="1242" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1242" t="s">
-        <v>1942</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="1243" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1243" t="s">
-        <v>1195</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="1244" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1244" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="1245" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1245" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="1246" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1246" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="1247" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1247" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="1248" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1248" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="1249" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1249" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="1250" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1250" t="s">
-        <v>1932</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="1251" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1251" t="s">
-        <v>1933</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="1252" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1252" t="s">
-        <v>1202</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="1253" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1253" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="1254" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1254" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="1255" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1255" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="1256" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1256" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="1257" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1257" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="1258" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1258" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="1259" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1259" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="1260" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1260" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="1261" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1261" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1262" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1262" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="1263" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1263" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="1264" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1264" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="1265" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1265" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="1266" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1266" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="1267" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1267" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="1268" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1268" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="1269" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1269" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="1270" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1270" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="1271" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1271" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="1272" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1272" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="1273" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1273" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="1274" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1274" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="1275" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1275" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="1276" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1276" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="1277" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1277" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="1278" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1278" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="1279" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1279" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="1280" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1280" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="1281" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1281" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="1282" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1282" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="1283" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1283" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="1284" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1284" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="1285" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1285" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="1286" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1286" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="1287" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1287" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="1288" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1288" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="1289" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1289" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="1290" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1290" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="1291" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1291" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="1292" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1292" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="1293" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1293" t="s">
-        <v>1242</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="1294" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1294" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="1295" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1295" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="1296" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1296" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="1297" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1297" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="1298" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1298" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="1299" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1299" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="1300" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1300" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="1301" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1301" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1302" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1302" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="1303" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1303" t="s">
-        <v>1251</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="1304" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1304" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="1305" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1305" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="1306" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1306" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="1307" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1307" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="1308" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1308" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="1309" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1309" t="s">
-        <v>1258</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="1310" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1310" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="1311" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1311" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="1312" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1312" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="1313" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1313" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="1314" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1314" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="1315" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1315" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1316" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1316" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="1317" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1317" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1318" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1318" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="1319" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1319" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1320" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1320" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1321" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1321" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="1322" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1322" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="1323" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1323" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="1324" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1324" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="1325" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1325" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="1326" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1326" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="1327" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1327" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="1328" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1328" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="1329" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1329" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="1330" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1330" t="s">
-        <v>1279</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1331" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1331" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="1332" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1332" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="1333" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1333" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="1334" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1334" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="1335" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1335" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="1336" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1336" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="1337" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1337" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="1338" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1338" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="1339" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1339" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="1340" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1340" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="1341" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1341" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1342" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1342" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="1343" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1343" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="1344" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1344" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="1345" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1345" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1346" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1346" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1347" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1347" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="1348" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1348" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="1349" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1349" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1350" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1350" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1351" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1351" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="1352" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1352" t="s">
-        <v>1318</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="1353" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1353" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="1354" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1354" t="s">
-        <v>1302</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="1355" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1355" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="1356" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1356" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1357" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1357" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="1358" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1358" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="1359" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1359" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="1360" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1360" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="1361" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1361" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="1362" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1362" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="1363" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1363" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="1364" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1364" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="1365" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1365" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="1366" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1366" t="s">
-        <v>1310</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="1367" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1367" t="s">
-        <v>1315</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="1368" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1368" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="1369" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1369" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="1370" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1370" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="1371" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1371" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="1372" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1372" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="1373" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1373" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="1374" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1374" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="1375" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1375" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="1376" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1376" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="1377" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1377" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="1378" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1378" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="1379" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1379" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="1380" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1380" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="1381" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1381" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="1382" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1382" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="1383" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1383" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="1384" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1384" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="1385" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1385" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="1386" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1386" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="1387" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1387" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="1388" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1388" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="1389" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1389" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="1390" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1390" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="1391" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1391" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1392" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1392" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="1393" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1393" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="1394" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1394" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1395" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1395" t="s">
-        <v>1342</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="1396" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1396" t="s">
-        <v>1934</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1397" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1397" t="s">
-        <v>1795</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="1398" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1398" t="s">
-        <v>1797</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="1399" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1399" t="s">
-        <v>1935</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="1400" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1400" t="s">
-        <v>1936</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="1401" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1401" t="s">
-        <v>1794</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="1402" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1402" t="s">
-        <v>1799</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="1403" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1403" t="s">
-        <v>1798</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="1404" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1404" t="s">
-        <v>1796</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="1405" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1405" t="s">
-        <v>1793</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="1406" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1406" t="s">
-        <v>1792</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="1407" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1407" t="s">
-        <v>1346</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="1408" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1408" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="1409" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1409" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="1410" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1410" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="1411" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1411" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="1412" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1412" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="1413" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1413" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="1414" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1414" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="1415" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1415" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="1416" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1416" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="1417" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1417" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="1418" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1418" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="1419" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1419" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="1420" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1420" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="1421" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1421" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="1422" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1422" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="1423" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1423" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="1424" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1424" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="1425" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1425" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="1426" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1426" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="1427" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1427" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="1428" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1428" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="1429" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1429" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="1430" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1430" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="1431" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1431" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="1432" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1432" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="1433" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1433" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="1434" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1434" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="1435" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1435" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="1436" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1436" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="1437" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1437" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="1438" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1438" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="1439" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1439" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="1440" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1440" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="1441" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1441" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="1442" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1442" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="1443" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1443" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="1444" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1444" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="1445" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1445" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="1446" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1446" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="1447" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1447" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="1448" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1448" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="1449" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1449" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="1450" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1450" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="1451" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1451" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1452" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1452" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="1453" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1453" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="1454" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1454" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="1455" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1455" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="1456" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1456" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="1457" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1457" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="1458" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1458" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="1459" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1459" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="1460" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1460" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="1461" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1461" t="s">
-        <v>1409</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="1462" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1462" t="s">
-        <v>1400</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="1463" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1463" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="1464" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1464" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="1465" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1465" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="1466" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1466" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="1467" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1467" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="1468" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1468" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="1469" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1469" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="1470" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1470" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="1471" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1471" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="1472" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1472" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="1473" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1473" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="1474" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1474" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="1475" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1475" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="1476" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1476" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="1477" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1477" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1478" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1478" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="1479" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1479" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="1480" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1480" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="1481" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1481" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="1482" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1482" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="1483" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1483" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="1484" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1484" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="1485" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1485" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="1486" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1486" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="1487" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1487" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1488" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1488" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="1489" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1489" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="1490" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1490" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1491" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1491" t="s">
-        <v>1428</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1492" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1492" t="s">
-        <v>1937</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="1493" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1493" t="s">
-        <v>1431</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="1494" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1494" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="1495" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1495" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="1496" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1496" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="1497" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1497" t="s">
-        <v>1938</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="1498" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1498" t="s">
-        <v>1435</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="1499" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1499" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1500" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1500" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="1501" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1501" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="1502" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1502" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="1503" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1503" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="1504" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1504" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="1505" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1505" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="1506" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1506" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="1507" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1507" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="1508" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1508" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="1509" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1509" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="1510" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1510" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="1511" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1511" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="1512" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1512" t="s">
-        <v>1465</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="1513" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1513" t="s">
-        <v>1450</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="1514" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1514" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="1515" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1515" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="1516" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1516" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="1517" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1517" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="1518" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1518" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="1519" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1519" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1520" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1520" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="1521" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1521" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="1522" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1522" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="1523" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1523" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="1524" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1524" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="1525" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1525" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="1526" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1526" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="1527" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1527" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="1528" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1528" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="1529" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1529" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1530" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1530" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="1531" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1531" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="1532" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1532" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="1533" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1533" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="1534" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1534" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="1535" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1535" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="1536" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1536" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="1537" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1537" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="1538" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1538" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="1539" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1539" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="1540" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1540" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="1541" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1541" t="s">
-        <v>1439</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="1542" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1542" t="s">
-        <v>1479</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="1543" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1543" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="1544" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1544" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="1545" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1545" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="1546" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1546" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="1547" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1547" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="1548" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1548" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="1549" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1549" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1550" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1550" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="1551" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1551" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="1552" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1552" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="1553" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1553" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="1554" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1554" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="1555" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1555" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="1556" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1556" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="1557" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1557" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="1558" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1558" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="1559" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1559" t="s">
-        <v>1801</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="1560" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1560" t="s">
-        <v>1496</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="1561" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1561" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="1562" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1562" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="1563" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1563" t="s">
-        <v>1503</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="1564" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1564" t="s">
-        <v>1499</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="1565" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1565" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="1566" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1566" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="1567" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1567" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="1568" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1568" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="1569" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1569" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="1570" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1570" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="1571" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1571" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="1572" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1572" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="1573" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1573" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="1574" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1574" t="s">
-        <v>1514</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="1575" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1575" t="s">
-        <v>1510</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="1576" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1576" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="1577" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1577" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="1578" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1578" t="s">
-        <v>1939</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="1579" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1579" t="s">
-        <v>1513</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="1580" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1580" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="1581" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1581" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="1582" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1582" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="1583" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1583" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="1584" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1584" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="1585" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1585" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="1586" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1586" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="1587" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1587" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="1588" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1588" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="1589" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1589" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="1590" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1590" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="1591" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1591" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="1592" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1592" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="1593" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1593" t="s">
-        <v>1530</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="1594" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1594" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="1595" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1595" t="s">
-        <v>1528</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="1596" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1596" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="1597" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1597" t="s">
-        <v>1532</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="1598" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1598" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="1599" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1599" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1600" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1600" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="1601" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1601" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="1602" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1602" t="s">
-        <v>1540</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="1603" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1603" t="s">
-        <v>1536</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="1604" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1604" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="1605" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1605" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="1606" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1606" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="1607" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1607" t="s">
-        <v>1940</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="1608" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1608" t="s">
-        <v>1542</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="1609" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1609" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="1610" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1610" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="1611" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1611" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="1612" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1612" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="1613" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1613" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="1614" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1614" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="1615" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1615" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="1616" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1616" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="1617" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1617" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="1618" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1618" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="1619" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1619" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="1620" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1620" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="1621" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1621" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="1622" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1622" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="1623" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1623" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="1624" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1624" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="1625" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1625" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="1626" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1626" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="1627" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1627" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="1628" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1628" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="1629" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1629" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="1630" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1630" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="1631" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1631" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="1632" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1632" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="1633" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1633" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1634" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1634" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="1635" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1635" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="1636" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1636" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="1637" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1637" t="s">
-        <v>1943</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="1638" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1638" t="s">
-        <v>1571</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="1639" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1639" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="1640" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1640" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="1641" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1641" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="1642" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1642" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="1643" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1643" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="1644" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1644" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="1645" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1645" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="1646" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1646" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="1647" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1647" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="1648" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1648" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="1649" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1649" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="1650" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1650" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="1651" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1651" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="1652" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1652" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="1653" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1653" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="1654" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1654" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="1655" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1655" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="1656" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1656" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="1657" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1657" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="1658" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1658" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="1659" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1659" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="1660" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1660" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="1661" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1661" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="1662" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1662" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="1663" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1663" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="1664" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1664" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="1665" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1665" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="1666" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1666" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="1667" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1667" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="1668" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1668" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="1669" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1669" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="1670" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1670" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="1671" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1671" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="1672" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1672" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="1673" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1673" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="1674" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1674" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="1675" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1675" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="1676" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1676" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="1677" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1677" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="1678" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1678" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="1679" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1679" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="1680" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1680" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="1681" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1681" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="1682" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1682" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="1683" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1683" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="1684" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1684" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="1685" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1685" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="1686" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1686" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="1687" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1687" t="s">
-        <v>1941</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="1688" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1688" t="s">
-        <v>1620</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="1689" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1689" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="1690" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1690" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="1691" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1691" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="1692" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1692" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="1693" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1693" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="1694" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1694" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="1695" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1695" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="1696" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1696" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="1697" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1697" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="1698" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1698" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="1699" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1699" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="1700" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1700" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="1701" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1701" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="1702" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1702" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="1703" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1703" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="1704" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1704" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="1705" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1705" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="1706" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1706" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="1707" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1707" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="1708" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1708" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="1709" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1709" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="1710" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1710" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="1711" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1711" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="1712" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1712" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="1713" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1713" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="1714" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1714" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="1715" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1715" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="1716" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1716" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="1717" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1717" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="1718" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1718" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="1719" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1719" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="1720" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1720" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="1721" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1721" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="1722" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1722" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="1723" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1723" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="1724" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1724" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="1725" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1725" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="1726" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1726" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="1727" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1727" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="1728" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1728" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="1729" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1729" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="1730" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1730" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="1731" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1731" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1732" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1732" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="1733" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1733" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="1734" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1734" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="1735" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1735" t="s">
-        <v>1669</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="1736" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1736" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="1737" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1737" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="1738" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1738" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="1739" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1739" t="s">
-        <v>1666</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="1740" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1740" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="1741" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1741" t="s">
-        <v>1673</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="1742" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1742" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="1743" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1743" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="1744" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1744" t="s">
-        <v>1677</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="1745" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1745" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="1746" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1746" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="1747" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1747" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="1748" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1748" t="s">
-        <v>1682</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="1749" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1749" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="1750" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1750" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="1751" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1751" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="1752" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1752" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="1753" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1753" t="s">
-        <v>1690</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="1754" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1754" t="s">
-        <v>1680</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="1755" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1755" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="1756" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1756" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="1757" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1757" t="s">
-        <v>1688</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="1758" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1758" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="1759" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1759" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="1760" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1760" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="1761" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C1761" t="s">
         <v>1692</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregar CCNN en plantilla capacitación participantes.
</commit_message>
<xml_diff>
--- a/SIGOFCv3/Archivos/Plantilla/CapacitacionParticipantes_v3.xlsx
+++ b/SIGOFCv3/Archivos/Plantilla/CapacitacionParticipantes_v3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20405"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC62A2F8-3028-412D-A566-1CEB651497CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19270BB2-3F86-463C-B744-F23AF3E4FC57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2020" uniqueCount="1945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="1946">
   <si>
     <t>OBSERVACION</t>
   </si>
@@ -5864,6 +5864,9 @@
   </si>
   <si>
     <t>San Martin de Porres (LORETO-PUTUMAYO-TENIENTE MANUEL CLAVERO)</t>
+  </si>
+  <si>
+    <t>Tsimepanko (UCAYALI-ATALAYA-TAHUANÍA)</t>
   </si>
 </sst>
 </file>
@@ -6405,10 +6408,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E1761"/>
+  <dimension ref="A1:E1762"/>
   <sheetViews>
-    <sheetView topLeftCell="A1722" workbookViewId="0">
-      <selection activeCell="C1117" sqref="C1117"/>
+    <sheetView topLeftCell="A1740" workbookViewId="0">
+      <selection activeCell="C1587" sqref="C1587"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14731,881 +14734,886 @@
     </row>
     <row r="1586" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1586" t="s">
-        <v>1520</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="1587" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1587" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="1588" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1588" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="1589" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1589" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="1590" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1590" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="1591" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1591" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="1592" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1592" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="1593" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1593" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="1594" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1594" t="s">
-        <v>1530</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="1595" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1595" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="1596" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1596" t="s">
-        <v>1528</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="1597" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1597" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="1598" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1598" t="s">
-        <v>1532</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="1599" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1599" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="1600" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1600" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1601" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1601" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="1602" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1602" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="1603" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1603" t="s">
-        <v>1540</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="1604" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1604" t="s">
-        <v>1536</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="1605" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1605" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="1606" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1606" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="1607" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1607" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="1608" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1608" t="s">
-        <v>1939</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="1609" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1609" t="s">
-        <v>1542</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="1610" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1610" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="1611" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1611" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="1612" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1612" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="1613" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1613" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="1614" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1614" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="1615" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1615" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="1616" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1616" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="1617" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1617" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="1618" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1618" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="1619" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1619" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="1620" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1620" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="1621" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1621" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="1622" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1622" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="1623" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1623" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="1624" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1624" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="1625" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1625" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="1626" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1626" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="1627" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1627" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="1628" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1628" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="1629" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1629" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="1630" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1630" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="1631" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1631" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="1632" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1632" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="1633" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1633" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="1634" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1634" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1635" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1635" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="1636" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1636" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="1637" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1637" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="1638" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1638" t="s">
-        <v>1942</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="1639" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1639" t="s">
-        <v>1571</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="1640" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1640" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="1641" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1641" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="1642" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1642" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="1643" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1643" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="1644" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1644" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="1645" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1645" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="1646" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1646" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="1647" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1647" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="1648" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1648" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="1649" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1649" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="1650" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1650" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="1651" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1651" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="1652" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1652" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="1653" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1653" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="1654" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1654" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="1655" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1655" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="1656" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1656" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="1657" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1657" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="1658" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1658" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="1659" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1659" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="1660" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1660" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="1661" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1661" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="1662" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1662" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="1663" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1663" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="1664" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1664" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="1665" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1665" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="1666" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1666" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="1667" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1667" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="1668" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1668" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="1669" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1669" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="1670" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1670" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="1671" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1671" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="1672" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1672" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="1673" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1673" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="1674" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1674" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="1675" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1675" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="1676" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1676" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="1677" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1677" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="1678" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1678" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="1679" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1679" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="1680" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1680" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="1681" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1681" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="1682" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1682" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="1683" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1683" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="1684" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1684" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="1685" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1685" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="1686" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1686" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="1687" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1687" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="1688" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1688" t="s">
-        <v>1940</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="1689" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1689" t="s">
-        <v>1620</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="1690" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1690" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="1691" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1691" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="1692" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1692" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="1693" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1693" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="1694" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1694" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="1695" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1695" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="1696" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1696" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="1697" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1697" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="1698" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1698" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="1699" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1699" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="1700" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1700" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="1701" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1701" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="1702" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1702" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="1703" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1703" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="1704" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1704" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="1705" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1705" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="1706" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1706" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="1707" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1707" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="1708" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1708" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="1709" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1709" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="1710" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1710" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="1711" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1711" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="1712" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1712" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="1713" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1713" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="1714" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1714" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="1715" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1715" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="1716" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1716" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="1717" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1717" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="1718" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1718" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="1719" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1719" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="1720" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1720" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="1721" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1721" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="1722" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1722" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="1723" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1723" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="1724" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1724" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="1725" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1725" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="1726" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1726" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="1727" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1727" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="1728" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1728" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="1729" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1729" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="1730" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1730" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="1731" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1731" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="1732" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1732" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1733" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1733" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="1734" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1734" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="1735" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1735" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="1736" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1736" t="s">
-        <v>1669</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="1737" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1737" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="1738" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1738" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="1739" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1739" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="1740" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1740" t="s">
-        <v>1666</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="1741" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1741" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="1742" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1742" t="s">
-        <v>1673</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="1743" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1743" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="1744" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1744" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="1745" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1745" t="s">
-        <v>1677</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="1746" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1746" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="1747" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1747" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="1748" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1748" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="1749" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1749" t="s">
-        <v>1682</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="1750" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1750" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="1751" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1751" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="1752" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1752" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="1753" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1753" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="1754" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1754" t="s">
-        <v>1690</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="1755" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1755" t="s">
-        <v>1680</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="1756" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1756" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="1757" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1757" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="1758" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1758" t="s">
-        <v>1688</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="1759" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1759" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="1760" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1760" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="1761" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C1761" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="1762" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C1762" t="s">
         <v>1692</v>
       </c>
     </row>

</xml_diff>